<commit_message>
updates for number of animals difference
</commit_message>
<xml_diff>
--- a/init_Synopsis_Dbdb.xlsx
+++ b/init_Synopsis_Dbdb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipzach\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipzach\Documents\MATLAB\Diabetes-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD374BC1-52D7-4837-97F2-A83BFE52E185}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922A9D68-A5AF-42E7-B9B9-E472EA90309E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animal" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="150">
   <si>
     <t>surgeon</t>
   </si>
@@ -460,6 +460,21 @@
   </si>
   <si>
     <t>SLM</t>
+  </si>
+  <si>
+    <t>Animal list #</t>
+  </si>
+  <si>
+    <t>New folder name</t>
+  </si>
+  <si>
+    <t>SWRLTDIdx is empty/missing</t>
+  </si>
+  <si>
+    <t>SWRLTDIdx is empty/missing, LFP is missing</t>
+  </si>
+  <si>
+    <t>Data Analysis Error list</t>
   </si>
 </sst>
 </file>
@@ -537,7 +552,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -568,6 +583,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -589,7 +616,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -685,6 +712,44 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1027,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:T85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70:N79"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1045,7 +1110,9 @@
     <col min="9" max="9" width="5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0.7109375" customWidth="1"/>
     <col min="11" max="11" width="5.28515625" customWidth="1"/>
-    <col min="12" max="1009" width="12.42578125" customWidth="1"/>
+    <col min="12" max="17" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="39" customWidth="1"/>
+    <col min="19" max="1009" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1482,7 +1549,7 @@
         <v>44104</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" ref="G15:G18" si="4">DAYS360(D18,F18)/7</f>
+        <f t="shared" ref="G18" si="4">DAYS360(D18,F18)/7</f>
         <v>28.428571428571427</v>
       </c>
       <c r="H18" s="25" t="s">
@@ -1493,7 +1560,7 @@
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="28">
-        <f t="shared" ref="K15:K18" si="5">G18*7</f>
+        <f t="shared" ref="K18" si="5">G18*7</f>
         <v>199</v>
       </c>
       <c r="M18" t="s">
@@ -1558,7 +1625,7 @@
         <v>44125</v>
       </c>
       <c r="G20" s="15">
-        <f t="shared" ref="G20:G22" si="8">DAYS360(D20,F20)/7</f>
+        <f t="shared" ref="G20:G21" si="8">DAYS360(D20,F20)/7</f>
         <v>52.571428571428569</v>
       </c>
       <c r="H20" s="16" t="s">
@@ -1569,7 +1636,7 @@
       </c>
       <c r="J20" s="19"/>
       <c r="K20" s="18">
-        <f t="shared" ref="K20:K22" si="9">G20*7</f>
+        <f t="shared" ref="K20:K21" si="9">G20*7</f>
         <v>368</v>
       </c>
       <c r="M20" t="s">
@@ -1710,7 +1777,7 @@
         <v>44141</v>
       </c>
       <c r="G24" s="15">
-        <f t="shared" ref="G23:G24" si="10">DAYS360(D24,F24)/7</f>
+        <f t="shared" ref="G24" si="10">DAYS360(D24,F24)/7</f>
         <v>55.857142857142854</v>
       </c>
       <c r="H24" s="16" t="s">
@@ -1721,7 +1788,7 @@
       </c>
       <c r="J24" s="19"/>
       <c r="K24" s="18">
-        <f t="shared" ref="K23:K24" si="11">G24*7</f>
+        <f t="shared" ref="K24" si="11">G24*7</f>
         <v>391</v>
       </c>
       <c r="M24" t="s">
@@ -1824,7 +1891,7 @@
         <v>44151</v>
       </c>
       <c r="G27" s="24">
-        <f t="shared" ref="G27:G30" si="16">DAYS360(D27,F27)/7</f>
+        <f t="shared" ref="G27:G28" si="16">DAYS360(D27,F27)/7</f>
         <v>28.571428571428573</v>
       </c>
       <c r="H27" s="25" t="s">
@@ -1835,7 +1902,7 @@
       </c>
       <c r="J27" s="27"/>
       <c r="K27" s="28">
-        <f t="shared" ref="K27:K30" si="17">G27*7</f>
+        <f t="shared" ref="K27:K28" si="17">G27*7</f>
         <v>200</v>
       </c>
       <c r="M27" t="s">
@@ -2032,7 +2099,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33" s="38" t="s">
         <v>112</v>
       </c>
@@ -2070,7 +2137,10 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
+      <c r="M34" t="s">
+        <v>146</v>
+      </c>
       <c r="N34" t="s">
         <v>142</v>
       </c>
@@ -2080,8 +2150,11 @@
       <c r="P34" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="29" t="s">
         <v>37</v>
       </c>
@@ -2112,7 +2185,7 @@
       </c>
       <c r="J35" s="36"/>
       <c r="K35" s="36">
-        <f>G35*7</f>
+        <f t="shared" ref="K35:K44" si="23">G35*7</f>
         <v>462</v>
       </c>
       <c r="L35" s="5"/>
@@ -2129,7 +2202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17">
       <c r="A36" s="29" t="s">
         <v>38</v>
       </c>
@@ -2160,7 +2233,7 @@
       </c>
       <c r="J36" s="37"/>
       <c r="K36" s="36">
-        <f>G36*7</f>
+        <f t="shared" si="23"/>
         <v>411</v>
       </c>
       <c r="M36" t="s">
@@ -2176,7 +2249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17">
       <c r="A37" s="29" t="s">
         <v>39</v>
       </c>
@@ -2207,7 +2280,7 @@
       </c>
       <c r="J37" s="37"/>
       <c r="K37" s="36">
-        <f>G37*7</f>
+        <f t="shared" si="23"/>
         <v>337</v>
       </c>
       <c r="M37" t="s">
@@ -2223,7 +2296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:17">
       <c r="A38" s="38" t="s">
         <v>54</v>
       </c>
@@ -2243,7 +2316,7 @@
         <v>44099</v>
       </c>
       <c r="G38" s="42">
-        <f>DAYS360(D38,F38)/7</f>
+        <f t="shared" ref="G38:G44" si="24">DAYS360(D38,F38)/7</f>
         <v>28.857142857142858</v>
       </c>
       <c r="H38" s="43" t="s">
@@ -2254,7 +2327,7 @@
       </c>
       <c r="J38" s="45"/>
       <c r="K38" s="46">
-        <f>G38*7</f>
+        <f t="shared" si="23"/>
         <v>202</v>
       </c>
       <c r="M38" t="s">
@@ -2270,7 +2343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:17">
       <c r="A39" s="38" t="s">
         <v>55</v>
       </c>
@@ -2290,7 +2363,7 @@
         <v>44099</v>
       </c>
       <c r="G39" s="42">
-        <f>DAYS360(D39,F39)/7</f>
+        <f t="shared" si="24"/>
         <v>28.857142857142858</v>
       </c>
       <c r="H39" s="43" t="s">
@@ -2301,7 +2374,7 @@
       </c>
       <c r="J39" s="45"/>
       <c r="K39" s="46">
-        <f>G39*7</f>
+        <f t="shared" si="23"/>
         <v>202</v>
       </c>
       <c r="M39" t="s">
@@ -2317,7 +2390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:17">
       <c r="A40" s="38" t="s">
         <v>56</v>
       </c>
@@ -2337,7 +2410,7 @@
         <v>44103</v>
       </c>
       <c r="G40" s="42">
-        <f>DAYS360(D40,F40)/7</f>
+        <f t="shared" si="24"/>
         <v>28.285714285714285</v>
       </c>
       <c r="H40" s="43" t="s">
@@ -2348,7 +2421,7 @@
       </c>
       <c r="J40" s="45"/>
       <c r="K40" s="46">
-        <f>G40*7</f>
+        <f t="shared" si="23"/>
         <v>198</v>
       </c>
       <c r="M40" t="s">
@@ -2364,7 +2437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:17">
       <c r="A41" s="29" t="s">
         <v>90</v>
       </c>
@@ -2384,7 +2457,7 @@
         <v>44127</v>
       </c>
       <c r="G41" s="33">
-        <f>DAYS360(D41,F41)/7</f>
+        <f t="shared" si="24"/>
         <v>52.142857142857146</v>
       </c>
       <c r="H41" s="34" t="s">
@@ -2395,7 +2468,7 @@
       </c>
       <c r="J41" s="37"/>
       <c r="K41" s="36">
-        <f>G41*7</f>
+        <f t="shared" si="23"/>
         <v>365</v>
       </c>
       <c r="M41" t="s">
@@ -2411,7 +2484,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17">
       <c r="A42" s="29" t="s">
         <v>94</v>
       </c>
@@ -2431,7 +2504,7 @@
         <v>44134</v>
       </c>
       <c r="G42" s="33">
-        <f>DAYS360(D42,F42)/7</f>
+        <f t="shared" si="24"/>
         <v>53.142857142857146</v>
       </c>
       <c r="H42" s="34" t="s">
@@ -2442,7 +2515,7 @@
       </c>
       <c r="J42" s="37"/>
       <c r="K42" s="36">
-        <f>G42*7</f>
+        <f t="shared" si="23"/>
         <v>372</v>
       </c>
       <c r="M42" t="s">
@@ -2458,7 +2531,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:17">
       <c r="A43" s="38" t="s">
         <v>106</v>
       </c>
@@ -2478,7 +2551,7 @@
         <v>44152</v>
       </c>
       <c r="G43" s="42">
-        <f>DAYS360(D43,F43)/7</f>
+        <f t="shared" si="24"/>
         <v>27.428571428571427</v>
       </c>
       <c r="H43" s="43" t="s">
@@ -2489,7 +2562,7 @@
       </c>
       <c r="J43" s="45"/>
       <c r="K43" s="46">
-        <f>G43*7</f>
+        <f t="shared" si="23"/>
         <v>192</v>
       </c>
       <c r="M43" t="s">
@@ -2505,7 +2578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:17">
       <c r="A44" s="38" t="s">
         <v>107</v>
       </c>
@@ -2525,7 +2598,7 @@
         <v>44152</v>
       </c>
       <c r="G44" s="42">
-        <f>DAYS360(D44,F44)/7</f>
+        <f t="shared" si="24"/>
         <v>29.571428571428573</v>
       </c>
       <c r="H44" s="43" t="s">
@@ -2536,7 +2609,7 @@
       </c>
       <c r="J44" s="45"/>
       <c r="K44" s="46">
-        <f>G44*7</f>
+        <f t="shared" si="23"/>
         <v>207</v>
       </c>
       <c r="M44" t="s">
@@ -2552,7 +2625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:17">
       <c r="A45" s="38" t="s">
         <v>111</v>
       </c>
@@ -2572,7 +2645,7 @@
         <v>44159</v>
       </c>
       <c r="G45" s="42">
-        <f t="shared" ref="G45:G59" si="23">DAYS360(D45,F45)/7</f>
+        <f t="shared" ref="G45:G59" si="25">DAYS360(D45,F45)/7</f>
         <v>26.571428571428573</v>
       </c>
       <c r="H45" s="43" t="s">
@@ -2583,7 +2656,7 @@
       </c>
       <c r="J45" s="45"/>
       <c r="K45" s="46">
-        <f t="shared" ref="K45:K59" si="24">G45*7</f>
+        <f t="shared" ref="K45:K59" si="26">G45*7</f>
         <v>186</v>
       </c>
       <c r="M45" t="s">
@@ -2599,7 +2672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:17">
       <c r="A46" s="38" t="s">
         <v>112</v>
       </c>
@@ -2619,7 +2692,7 @@
         <v>44159</v>
       </c>
       <c r="G46" s="42">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>26.571428571428573</v>
       </c>
       <c r="H46" s="43" t="s">
@@ -2630,7 +2703,7 @@
       </c>
       <c r="J46" s="45"/>
       <c r="K46" s="46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>186</v>
       </c>
       <c r="M46" t="s">
@@ -2646,7 +2719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:17">
       <c r="A47" s="20" t="s">
         <v>51</v>
       </c>
@@ -2666,7 +2739,7 @@
         <v>44095</v>
       </c>
       <c r="G47" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.285714285714285</v>
       </c>
       <c r="H47" s="25" t="s">
@@ -2677,7 +2750,7 @@
       </c>
       <c r="J47" s="27"/>
       <c r="K47" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>198</v>
       </c>
       <c r="M47" t="s">
@@ -2693,7 +2766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:17">
       <c r="A48" s="20" t="s">
         <v>52</v>
       </c>
@@ -2713,7 +2786,7 @@
         <v>44097</v>
       </c>
       <c r="G48" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H48" s="25" t="s">
@@ -2724,7 +2797,7 @@
       </c>
       <c r="J48" s="27"/>
       <c r="K48" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>200</v>
       </c>
       <c r="M48" t="s">
@@ -2740,7 +2813,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:20">
       <c r="A49" s="20" t="s">
         <v>53</v>
       </c>
@@ -2760,7 +2833,7 @@
         <v>44097</v>
       </c>
       <c r="G49" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H49" s="25" t="s">
@@ -2771,7 +2844,7 @@
       </c>
       <c r="J49" s="27"/>
       <c r="K49" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>200</v>
       </c>
       <c r="M49" t="s">
@@ -2787,7 +2860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:20">
       <c r="A50" s="20" t="s">
         <v>57</v>
       </c>
@@ -2807,7 +2880,7 @@
         <v>44104</v>
       </c>
       <c r="G50" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.428571428571427</v>
       </c>
       <c r="H50" s="25" t="s">
@@ -2818,7 +2891,7 @@
       </c>
       <c r="J50" s="27"/>
       <c r="K50" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>199</v>
       </c>
       <c r="M50" t="s">
@@ -2834,7 +2907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:20">
       <c r="A51" s="20" t="s">
         <v>58</v>
       </c>
@@ -2854,7 +2927,7 @@
         <v>44104</v>
       </c>
       <c r="G51" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.428571428571427</v>
       </c>
       <c r="H51" s="25" t="s">
@@ -2865,7 +2938,7 @@
       </c>
       <c r="J51" s="27"/>
       <c r="K51" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>199</v>
       </c>
       <c r="M51" t="s">
@@ -2881,7 +2954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:20">
       <c r="A52" s="11" t="s">
         <v>84</v>
       </c>
@@ -2901,7 +2974,7 @@
         <v>44125</v>
       </c>
       <c r="G52" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>52.571428571428569</v>
       </c>
       <c r="H52" s="16" t="s">
@@ -2912,7 +2985,7 @@
       </c>
       <c r="J52" s="19"/>
       <c r="K52" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>368</v>
       </c>
       <c r="M52" t="s">
@@ -2928,7 +3001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:20">
       <c r="A53" s="11" t="s">
         <v>87</v>
       </c>
@@ -2948,7 +3021,7 @@
         <v>44126</v>
       </c>
       <c r="G53" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>52</v>
       </c>
       <c r="H53" s="16" t="s">
@@ -2959,7 +3032,7 @@
       </c>
       <c r="J53" s="19"/>
       <c r="K53" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>364</v>
       </c>
       <c r="M53" t="s">
@@ -2975,7 +3048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:20">
       <c r="A54" s="11" t="s">
         <v>96</v>
       </c>
@@ -2995,7 +3068,7 @@
         <v>44141</v>
       </c>
       <c r="G54" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>55.857142857142854</v>
       </c>
       <c r="H54" s="16" t="s">
@@ -3006,7 +3079,7 @@
       </c>
       <c r="J54" s="19"/>
       <c r="K54" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>391</v>
       </c>
       <c r="M54" t="s">
@@ -3022,7 +3095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:20">
       <c r="A55" s="11" t="s">
         <v>98</v>
       </c>
@@ -3042,7 +3115,7 @@
         <v>44145</v>
       </c>
       <c r="G55" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>59.142857142857146</v>
       </c>
       <c r="H55" s="16" t="s">
@@ -3053,7 +3126,7 @@
       </c>
       <c r="J55" s="19"/>
       <c r="K55" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>414</v>
       </c>
       <c r="M55" t="s">
@@ -3069,7 +3142,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:20">
       <c r="A56" s="11" t="s">
         <v>99</v>
       </c>
@@ -3089,7 +3162,7 @@
         <v>44145</v>
       </c>
       <c r="G56" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>60.285714285714285</v>
       </c>
       <c r="H56" s="16" t="s">
@@ -3100,7 +3173,7 @@
       </c>
       <c r="J56" s="19"/>
       <c r="K56" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>422</v>
       </c>
       <c r="M56" t="s">
@@ -3116,7 +3189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:20">
       <c r="A57" s="20" t="s">
         <v>102</v>
       </c>
@@ -3136,7 +3209,7 @@
         <v>44151</v>
       </c>
       <c r="G57" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H57" s="25" t="s">
@@ -3147,7 +3220,7 @@
       </c>
       <c r="J57" s="27"/>
       <c r="K57" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>200</v>
       </c>
       <c r="M57" t="s">
@@ -3163,7 +3236,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:20">
       <c r="A58" s="20" t="s">
         <v>103</v>
       </c>
@@ -3183,7 +3256,7 @@
         <v>44151</v>
       </c>
       <c r="G58" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H58" s="25" t="s">
@@ -3194,7 +3267,7 @@
       </c>
       <c r="J58" s="27"/>
       <c r="K58" s="28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>200</v>
       </c>
       <c r="M58" t="s">
@@ -3210,7 +3283,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:20">
       <c r="A59" s="11" t="s">
         <v>110</v>
       </c>
@@ -3230,7 +3303,7 @@
         <v>44158</v>
       </c>
       <c r="G59" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>53.285714285714285</v>
       </c>
       <c r="H59" s="16" t="s">
@@ -3241,7 +3314,7 @@
       </c>
       <c r="J59" s="19"/>
       <c r="K59" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>373</v>
       </c>
       <c r="M59" t="s">
@@ -3257,572 +3330,675 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
-      <c r="A61" s="38" t="s">
+    <row r="60" spans="1:20">
+      <c r="N60" t="s">
+        <v>142</v>
+      </c>
+      <c r="O60" t="s">
+        <v>143</v>
+      </c>
+      <c r="P60" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>145</v>
+      </c>
+      <c r="R60" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
+      <c r="A61" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="39" t="s">
+      <c r="B61" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="39" t="s">
+      <c r="C61" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D61" s="40">
+      <c r="D61" s="49">
         <v>43893</v>
       </c>
-      <c r="E61" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F61" s="40">
+      <c r="E61" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F61" s="49">
         <v>44099</v>
       </c>
-      <c r="G61" s="42">
+      <c r="G61" s="51">
         <f>DAYS360(D61,F61)/7</f>
         <v>28.857142857142858</v>
       </c>
-      <c r="H61" s="43" t="s">
+      <c r="H61" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I61" s="44">
+      <c r="I61" s="53">
         <v>32</v>
       </c>
-      <c r="J61" s="45"/>
-      <c r="K61" s="46">
+      <c r="J61" s="54"/>
+      <c r="K61" s="55">
         <f>G61*7</f>
         <v>202</v>
       </c>
-      <c r="M61" t="s">
+      <c r="L61" s="54"/>
+      <c r="M61" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="N61">
+      <c r="N61" s="54">
         <v>5</v>
       </c>
-      <c r="O61">
+      <c r="O61" s="54">
         <v>9</v>
       </c>
-      <c r="P61">
+      <c r="P61" s="54">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="1:16">
-      <c r="A62" s="38" t="s">
+      <c r="Q61" s="54">
+        <v>3</v>
+      </c>
+      <c r="R61" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="S61" s="54">
+        <v>7</v>
+      </c>
+      <c r="T61" s="54"/>
+    </row>
+    <row r="62" spans="1:20">
+      <c r="A62" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="39" t="s">
+      <c r="B62" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="C62" s="39" t="s">
+      <c r="C62" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D62" s="40">
+      <c r="D62" s="49">
         <v>43893</v>
       </c>
-      <c r="E62" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F62" s="40">
+      <c r="E62" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F62" s="49">
         <v>44099</v>
       </c>
-      <c r="G62" s="42">
+      <c r="G62" s="51">
         <f>DAYS360(D62,F62)/7</f>
         <v>28.857142857142858</v>
       </c>
-      <c r="H62" s="43" t="s">
+      <c r="H62" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I62" s="44">
+      <c r="I62" s="53">
         <v>34.5</v>
       </c>
-      <c r="J62" s="45"/>
-      <c r="K62" s="46">
+      <c r="J62" s="54"/>
+      <c r="K62" s="55">
         <f>G62*7</f>
         <v>202</v>
       </c>
-      <c r="M62" t="s">
+      <c r="L62" s="54"/>
+      <c r="M62" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="N62">
+      <c r="N62" s="54">
         <v>2</v>
       </c>
-      <c r="O62">
+      <c r="O62" s="54">
         <v>8</v>
       </c>
-      <c r="P62">
+      <c r="P62" s="54">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:16">
-      <c r="A63" s="38" t="s">
+      <c r="Q62" s="54">
+        <v>4</v>
+      </c>
+      <c r="R62" s="54"/>
+      <c r="S62" s="54"/>
+    </row>
+    <row r="63" spans="1:20">
+      <c r="A63" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="39" t="s">
+      <c r="B63" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="39" t="s">
+      <c r="C63" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D63" s="40">
+      <c r="D63" s="49">
         <v>43901</v>
       </c>
-      <c r="E63" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F63" s="40">
+      <c r="E63" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="49">
         <v>44103</v>
       </c>
-      <c r="G63" s="42">
+      <c r="G63" s="51">
         <f>DAYS360(D63,F63)/7</f>
         <v>28.285714285714285</v>
       </c>
-      <c r="H63" s="43" t="s">
+      <c r="H63" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I63" s="44">
+      <c r="I63" s="53">
         <v>32</v>
       </c>
-      <c r="J63" s="45"/>
-      <c r="K63" s="46">
+      <c r="J63" s="54"/>
+      <c r="K63" s="55">
         <f>G63*7</f>
         <v>198</v>
       </c>
-      <c r="M63" t="s">
+      <c r="L63" s="54"/>
+      <c r="M63" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="N63">
+      <c r="N63" s="54">
         <v>2</v>
       </c>
-      <c r="O63">
+      <c r="O63" s="54">
         <v>8</v>
       </c>
-      <c r="P63">
+      <c r="P63" s="54">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
-      <c r="A64" s="38" t="s">
+      <c r="Q63" s="54">
+        <v>5</v>
+      </c>
+      <c r="R63" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="S63" s="54"/>
+    </row>
+    <row r="64" spans="1:20">
+      <c r="A64" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B64" s="39" t="s">
+      <c r="B64" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C64" s="39" t="s">
+      <c r="C64" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D64" s="40">
+      <c r="D64" s="49">
         <v>43956</v>
       </c>
-      <c r="E64" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F64" s="40">
+      <c r="E64" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" s="49">
         <v>44152</v>
       </c>
-      <c r="G64" s="42">
+      <c r="G64" s="51">
         <f>DAYS360(D64,F64)/7</f>
         <v>27.428571428571427</v>
       </c>
-      <c r="H64" s="43" t="s">
+      <c r="H64" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I64" s="44">
+      <c r="I64" s="53">
         <v>47</v>
       </c>
-      <c r="J64" s="45"/>
-      <c r="K64" s="46">
+      <c r="J64" s="54"/>
+      <c r="K64" s="55">
         <f>G64*7</f>
         <v>192</v>
       </c>
-      <c r="M64" t="s">
+      <c r="L64" s="54"/>
+      <c r="M64" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="N64">
+      <c r="N64" s="54">
         <v>2</v>
       </c>
-      <c r="O64">
+      <c r="O64" s="54">
         <v>6</v>
       </c>
-      <c r="P64">
+      <c r="P64" s="54">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:16">
-      <c r="A65" s="38" t="s">
+      <c r="Q64" s="54">
+        <v>6</v>
+      </c>
+      <c r="R64" s="54"/>
+      <c r="S64" s="54"/>
+    </row>
+    <row r="65" spans="1:19">
+      <c r="A65" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="39" t="s">
+      <c r="B65" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="39" t="s">
+      <c r="C65" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D65" s="40">
+      <c r="D65" s="49">
         <v>43941</v>
       </c>
-      <c r="E65" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F65" s="40">
+      <c r="E65" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F65" s="49">
         <v>44152</v>
       </c>
-      <c r="G65" s="42">
+      <c r="G65" s="51">
         <f>DAYS360(D65,F65)/7</f>
         <v>29.571428571428573</v>
       </c>
-      <c r="H65" s="43" t="s">
+      <c r="H65" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I65" s="44">
+      <c r="I65" s="53">
         <v>32</v>
       </c>
-      <c r="J65" s="45"/>
-      <c r="K65" s="46">
+      <c r="J65" s="54"/>
+      <c r="K65" s="55">
         <f>G65*7</f>
         <v>207</v>
       </c>
-      <c r="M65" t="s">
+      <c r="L65" s="54"/>
+      <c r="M65" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="N65">
+      <c r="N65" s="54">
         <v>2</v>
       </c>
-      <c r="O65">
+      <c r="O65" s="54">
         <v>7</v>
       </c>
-      <c r="P65">
+      <c r="P65" s="54">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="38" t="s">
+      <c r="Q65" s="54">
+        <v>7</v>
+      </c>
+      <c r="R65" s="54"/>
+      <c r="S65" s="54"/>
+    </row>
+    <row r="66" spans="1:19">
+      <c r="A66" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="39" t="s">
+      <c r="B66" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="C66" s="39" t="s">
+      <c r="C66" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D66" s="40">
+      <c r="D66" s="49">
         <v>43969</v>
       </c>
-      <c r="E66" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F66" s="40">
+      <c r="E66" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" s="49">
         <v>44159</v>
       </c>
-      <c r="G66" s="42">
-        <f t="shared" ref="G66:G70" si="25">DAYS360(D66,F66)/7</f>
+      <c r="G66" s="51">
+        <f t="shared" ref="G66:G70" si="27">DAYS360(D66,F66)/7</f>
         <v>26.571428571428573</v>
       </c>
-      <c r="H66" s="43" t="s">
+      <c r="H66" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I66" s="44">
+      <c r="I66" s="53">
         <v>34</v>
       </c>
-      <c r="J66" s="45"/>
-      <c r="K66" s="46">
-        <f t="shared" ref="K66:K67" si="26">G66*7</f>
+      <c r="J66" s="54"/>
+      <c r="K66" s="55">
+        <f t="shared" ref="K66:K67" si="28">G66*7</f>
         <v>186</v>
       </c>
-      <c r="M66" t="s">
+      <c r="L66" s="54"/>
+      <c r="M66" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="N66">
+      <c r="N66" s="54">
         <v>2</v>
       </c>
-      <c r="O66">
+      <c r="O66" s="54">
         <v>7</v>
       </c>
-      <c r="P66">
+      <c r="P66" s="54">
         <v>14</v>
       </c>
-    </row>
-    <row r="67" spans="1:16">
-      <c r="A67" s="38" t="s">
+      <c r="Q66" s="54">
+        <v>8</v>
+      </c>
+      <c r="R66" s="54"/>
+      <c r="S66" s="54"/>
+    </row>
+    <row r="67" spans="1:19">
+      <c r="A67" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B67" s="39" t="s">
+      <c r="B67" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="C67" s="39" t="s">
+      <c r="C67" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="40">
+      <c r="D67" s="49">
         <v>43969</v>
       </c>
-      <c r="E67" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="F67" s="40">
+      <c r="E67" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F67" s="49">
         <v>44159</v>
       </c>
-      <c r="G67" s="42">
-        <f t="shared" si="25"/>
+      <c r="G67" s="51">
+        <f t="shared" si="27"/>
         <v>26.571428571428573</v>
       </c>
-      <c r="H67" s="43" t="s">
+      <c r="H67" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="I67" s="44">
+      <c r="I67" s="53">
         <v>40</v>
       </c>
-      <c r="J67" s="45"/>
-      <c r="K67" s="46">
-        <f t="shared" si="26"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="55">
+        <f t="shared" si="28"/>
         <v>186</v>
       </c>
-      <c r="M67" t="s">
+      <c r="L67" s="54"/>
+      <c r="M67" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="N67">
+      <c r="N67" s="54">
         <v>2</v>
       </c>
-      <c r="O67">
+      <c r="O67" s="54">
         <v>7</v>
       </c>
-      <c r="P67">
+      <c r="P67" s="54">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:16">
-      <c r="A68" s="29" t="s">
+      <c r="Q67" s="54">
+        <v>9</v>
+      </c>
+      <c r="R67" s="54"/>
+      <c r="S67" s="54"/>
+    </row>
+    <row r="68" spans="1:19">
+      <c r="A68" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="C68" s="30" t="s">
+      <c r="C68" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="31">
+      <c r="D68" s="58">
         <v>43614</v>
       </c>
-      <c r="E68" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F68" s="31">
+      <c r="E68" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F68" s="58">
         <v>44085</v>
       </c>
-      <c r="G68" s="33">
-        <f t="shared" si="25"/>
+      <c r="G68" s="60">
+        <f t="shared" si="27"/>
         <v>66</v>
       </c>
-      <c r="H68" s="34" t="s">
+      <c r="H68" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="35">
+      <c r="I68" s="62">
         <v>29.4</v>
       </c>
-      <c r="J68" s="36"/>
-      <c r="K68" s="36">
+      <c r="J68" s="63"/>
+      <c r="K68" s="63">
         <f>G68*7</f>
         <v>462</v>
       </c>
-      <c r="L68" s="5"/>
-      <c r="M68" s="5" t="s">
+      <c r="L68" s="63"/>
+      <c r="M68" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="N68">
+      <c r="N68" s="64">
         <v>5</v>
       </c>
-      <c r="O68">
+      <c r="O68" s="64">
         <v>10</v>
       </c>
-      <c r="P68">
+      <c r="P68" s="64">
         <v>14</v>
       </c>
-    </row>
-    <row r="69" spans="1:16">
-      <c r="A69" s="29" t="s">
+      <c r="Q68" s="64">
+        <v>10</v>
+      </c>
+      <c r="R68" s="64"/>
+      <c r="S68" s="64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
+      <c r="A69" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="30" t="s">
+      <c r="B69" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="C69" s="30" t="s">
+      <c r="C69" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D69" s="31">
+      <c r="D69" s="58">
         <v>43669</v>
       </c>
-      <c r="E69" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F69" s="31">
+      <c r="E69" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F69" s="58">
         <v>44088</v>
       </c>
-      <c r="G69" s="33">
-        <f t="shared" si="25"/>
+      <c r="G69" s="60">
+        <f t="shared" si="27"/>
         <v>58.714285714285715</v>
       </c>
-      <c r="H69" s="34" t="s">
+      <c r="H69" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="I69" s="35">
+      <c r="I69" s="62">
         <v>33.200000000000003</v>
       </c>
-      <c r="J69" s="37"/>
-      <c r="K69" s="36">
+      <c r="J69" s="64"/>
+      <c r="K69" s="63">
         <f>G69*7</f>
         <v>411</v>
       </c>
-      <c r="M69" t="s">
+      <c r="L69" s="64"/>
+      <c r="M69" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="N69">
+      <c r="N69" s="64">
         <v>4</v>
       </c>
-      <c r="O69">
+      <c r="O69" s="64">
         <v>9</v>
       </c>
-      <c r="P69">
+      <c r="P69" s="64">
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="1:16">
-      <c r="A70" s="29" t="s">
+      <c r="Q69" s="64">
+        <v>11</v>
+      </c>
+      <c r="R69" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="S69" s="64"/>
+    </row>
+    <row r="70" spans="1:19">
+      <c r="A70" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C70" s="30" t="s">
+      <c r="C70" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D70" s="31">
+      <c r="D70" s="58">
         <v>43747</v>
       </c>
-      <c r="E70" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F70" s="31">
+      <c r="E70" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" s="58">
         <v>44090</v>
       </c>
-      <c r="G70" s="33">
-        <f t="shared" si="25"/>
+      <c r="G70" s="60">
+        <f t="shared" si="27"/>
         <v>48.142857142857146</v>
       </c>
-      <c r="H70" s="34" t="s">
+      <c r="H70" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="I70" s="35">
-        <v>30</v>
-      </c>
-      <c r="J70" s="37"/>
-      <c r="K70" s="36">
+      <c r="I70" s="62">
+        <v>30</v>
+      </c>
+      <c r="J70" s="64"/>
+      <c r="K70" s="63">
         <f>G70*7</f>
         <v>337</v>
       </c>
-      <c r="M70" t="s">
+      <c r="L70" s="64"/>
+      <c r="M70" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="N70">
+      <c r="N70" s="64">
         <v>2</v>
       </c>
-      <c r="O70">
+      <c r="O70" s="64">
         <v>8</v>
       </c>
-      <c r="P70">
+      <c r="P70" s="64">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:16">
-      <c r="A71" s="29" t="s">
+      <c r="Q70" s="64">
+        <v>12</v>
+      </c>
+      <c r="R70" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="S70" s="64"/>
+    </row>
+    <row r="71" spans="1:19">
+      <c r="A71" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="B71" s="30" t="s">
+      <c r="B71" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="C71" s="30" t="s">
+      <c r="C71" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D71" s="31">
+      <c r="D71" s="58">
         <v>43756</v>
       </c>
-      <c r="E71" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F71" s="31">
+      <c r="E71" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F71" s="58">
         <v>44127</v>
       </c>
-      <c r="G71" s="33">
+      <c r="G71" s="60">
         <f>DAYS360(D71,F71)/7</f>
         <v>52.142857142857146</v>
       </c>
-      <c r="H71" s="34" t="s">
+      <c r="H71" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="I71" s="35">
+      <c r="I71" s="62">
         <v>31.6</v>
       </c>
-      <c r="J71" s="37"/>
-      <c r="K71" s="36">
+      <c r="J71" s="64"/>
+      <c r="K71" s="63">
         <f>G71*7</f>
         <v>365</v>
       </c>
-      <c r="M71" t="s">
+      <c r="L71" s="64"/>
+      <c r="M71" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="N71">
+      <c r="N71" s="64">
         <v>2</v>
       </c>
-      <c r="O71">
+      <c r="O71" s="64">
         <v>8</v>
       </c>
-      <c r="P71">
+      <c r="P71" s="64">
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:16">
-      <c r="A72" s="29" t="s">
+      <c r="Q71" s="64">
+        <v>13</v>
+      </c>
+      <c r="R71" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="S71" s="64"/>
+    </row>
+    <row r="72" spans="1:19">
+      <c r="A72" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="B72" s="30" t="s">
+      <c r="B72" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="30" t="s">
+      <c r="C72" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D72" s="31">
+      <c r="D72" s="58">
         <v>43756</v>
       </c>
-      <c r="E72" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F72" s="31">
+      <c r="E72" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F72" s="58">
         <v>44134</v>
       </c>
-      <c r="G72" s="33">
+      <c r="G72" s="60">
         <f>DAYS360(D72,F72)/7</f>
         <v>53.142857142857146</v>
       </c>
-      <c r="H72" s="34" t="s">
+      <c r="H72" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="I72" s="35">
+      <c r="I72" s="62">
         <v>30.4</v>
       </c>
-      <c r="J72" s="37"/>
-      <c r="K72" s="36">
+      <c r="J72" s="64"/>
+      <c r="K72" s="63">
         <f>G72*7</f>
         <v>372</v>
       </c>
-      <c r="M72" t="s">
+      <c r="L72" s="64"/>
+      <c r="M72" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="N72">
+      <c r="N72" s="64">
         <v>2</v>
       </c>
-      <c r="O72">
+      <c r="O72" s="64">
         <v>7</v>
       </c>
-      <c r="P72">
+      <c r="P72" s="64">
         <v>14</v>
       </c>
-    </row>
-    <row r="73" spans="1:16">
+      <c r="Q72" s="64">
+        <v>14</v>
+      </c>
+      <c r="R72" s="64"/>
+      <c r="S72" s="64"/>
+    </row>
+    <row r="73" spans="1:19">
       <c r="A73" s="20" t="s">
         <v>51</v>
       </c>
@@ -3842,7 +4018,7 @@
         <v>44095</v>
       </c>
       <c r="G73" s="24">
-        <f t="shared" ref="G73:G85" si="27">DAYS360(D73,F73)/7</f>
+        <f t="shared" ref="G73:G85" si="29">DAYS360(D73,F73)/7</f>
         <v>28.285714285714285</v>
       </c>
       <c r="H73" s="25" t="s">
@@ -3853,23 +4029,31 @@
       </c>
       <c r="J73" s="27"/>
       <c r="K73" s="28">
-        <f t="shared" ref="K73:K85" si="28">G73*7</f>
+        <f t="shared" ref="K73:K85" si="30">G73*7</f>
         <v>198</v>
       </c>
-      <c r="M73" t="s">
+      <c r="L73" s="27"/>
+      <c r="M73" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="N73">
+      <c r="N73" s="27">
         <v>2</v>
       </c>
-      <c r="O73">
+      <c r="O73" s="27">
         <v>8</v>
       </c>
-      <c r="P73">
+      <c r="P73" s="27">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:16">
+      <c r="Q73" s="27">
+        <v>15</v>
+      </c>
+      <c r="R73" s="27"/>
+      <c r="S73" s="27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19">
       <c r="A74" s="20" t="s">
         <v>52</v>
       </c>
@@ -3889,7 +4073,7 @@
         <v>44097</v>
       </c>
       <c r="G74" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H74" s="25" t="s">
@@ -3900,23 +4084,31 @@
       </c>
       <c r="J74" s="27"/>
       <c r="K74" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>200</v>
       </c>
-      <c r="M74" t="s">
+      <c r="L74" s="27"/>
+      <c r="M74" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="N74">
+      <c r="N74" s="27">
         <v>2</v>
       </c>
-      <c r="O74">
+      <c r="O74" s="27">
         <v>8</v>
       </c>
-      <c r="P74">
+      <c r="P74" s="27">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:16">
+      <c r="Q74" s="27">
+        <v>16</v>
+      </c>
+      <c r="R74" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="S74" s="27"/>
+    </row>
+    <row r="75" spans="1:19">
       <c r="A75" s="20" t="s">
         <v>53</v>
       </c>
@@ -3936,7 +4128,7 @@
         <v>44097</v>
       </c>
       <c r="G75" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H75" s="25" t="s">
@@ -3947,23 +4139,31 @@
       </c>
       <c r="J75" s="27"/>
       <c r="K75" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>200</v>
       </c>
-      <c r="M75" t="s">
+      <c r="L75" s="27"/>
+      <c r="M75" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="N75">
+      <c r="N75" s="27">
         <v>2</v>
       </c>
-      <c r="O75">
+      <c r="O75" s="27">
         <v>8</v>
       </c>
-      <c r="P75">
+      <c r="P75" s="27">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="Q75" s="27">
+        <v>17</v>
+      </c>
+      <c r="R75" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="S75" s="27"/>
+    </row>
+    <row r="76" spans="1:19">
       <c r="A76" s="20" t="s">
         <v>57</v>
       </c>
@@ -3983,7 +4183,7 @@
         <v>44104</v>
       </c>
       <c r="G76" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28.428571428571427</v>
       </c>
       <c r="H76" s="25" t="s">
@@ -3994,23 +4194,31 @@
       </c>
       <c r="J76" s="27"/>
       <c r="K76" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>199</v>
       </c>
-      <c r="M76" t="s">
+      <c r="L76" s="27"/>
+      <c r="M76" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="N76">
+      <c r="N76" s="27">
         <v>2</v>
       </c>
-      <c r="O76">
+      <c r="O76" s="27">
         <v>7</v>
       </c>
-      <c r="P76">
+      <c r="P76" s="27">
         <v>11</v>
       </c>
-    </row>
-    <row r="77" spans="1:16">
+      <c r="Q76" s="27">
+        <v>18</v>
+      </c>
+      <c r="R76" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="S76" s="27"/>
+    </row>
+    <row r="77" spans="1:19">
       <c r="A77" s="20" t="s">
         <v>58</v>
       </c>
@@ -4030,7 +4238,7 @@
         <v>44104</v>
       </c>
       <c r="G77" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28.428571428571427</v>
       </c>
       <c r="H77" s="25" t="s">
@@ -4041,23 +4249,29 @@
       </c>
       <c r="J77" s="27"/>
       <c r="K77" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>199</v>
       </c>
-      <c r="M77" t="s">
+      <c r="L77" s="27"/>
+      <c r="M77" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="N77">
+      <c r="N77" s="27">
         <v>2</v>
       </c>
-      <c r="O77">
+      <c r="O77" s="27">
         <v>8</v>
       </c>
-      <c r="P77">
+      <c r="P77" s="27">
         <v>14</v>
       </c>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="Q77" s="27">
+        <v>19</v>
+      </c>
+      <c r="R77" s="27"/>
+      <c r="S77" s="27"/>
+    </row>
+    <row r="78" spans="1:19">
       <c r="A78" s="20" t="s">
         <v>102</v>
       </c>
@@ -4077,7 +4291,7 @@
         <v>44151</v>
       </c>
       <c r="G78" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H78" s="25" t="s">
@@ -4088,23 +4302,29 @@
       </c>
       <c r="J78" s="27"/>
       <c r="K78" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>200</v>
       </c>
-      <c r="M78" t="s">
+      <c r="L78" s="27"/>
+      <c r="M78" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="N78">
+      <c r="N78" s="27">
         <v>2</v>
       </c>
-      <c r="O78">
+      <c r="O78" s="27">
         <v>9</v>
       </c>
-      <c r="P78">
+      <c r="P78" s="27">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:16">
+      <c r="Q78" s="27">
+        <v>20</v>
+      </c>
+      <c r="R78" s="27"/>
+      <c r="S78" s="27"/>
+    </row>
+    <row r="79" spans="1:19">
       <c r="A79" s="20" t="s">
         <v>103</v>
       </c>
@@ -4124,7 +4344,7 @@
         <v>44151</v>
       </c>
       <c r="G79" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>28.571428571428573</v>
       </c>
       <c r="H79" s="25" t="s">
@@ -4135,23 +4355,29 @@
       </c>
       <c r="J79" s="27"/>
       <c r="K79" s="28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>200</v>
       </c>
-      <c r="M79" t="s">
+      <c r="L79" s="27"/>
+      <c r="M79" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="N79">
+      <c r="N79" s="27">
         <v>2</v>
       </c>
-      <c r="O79">
+      <c r="O79" s="27">
         <v>7</v>
       </c>
-      <c r="P79">
+      <c r="P79" s="27">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="Q79" s="27">
+        <v>21</v>
+      </c>
+      <c r="R79" s="27"/>
+      <c r="S79" s="27"/>
+    </row>
+    <row r="80" spans="1:19">
       <c r="A80" s="11" t="s">
         <v>84</v>
       </c>
@@ -4171,7 +4397,7 @@
         <v>44125</v>
       </c>
       <c r="G80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>52.571428571428569</v>
       </c>
       <c r="H80" s="16" t="s">
@@ -4182,23 +4408,31 @@
       </c>
       <c r="J80" s="19"/>
       <c r="K80" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>368</v>
       </c>
-      <c r="M80" t="s">
+      <c r="L80" s="19"/>
+      <c r="M80" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="N80">
+      <c r="N80" s="19">
         <v>4</v>
       </c>
-      <c r="O80">
+      <c r="O80" s="19">
         <v>11</v>
       </c>
-      <c r="P80">
+      <c r="P80" s="19">
         <v>16</v>
       </c>
-    </row>
-    <row r="81" spans="1:16">
+      <c r="Q80" s="19">
+        <v>22</v>
+      </c>
+      <c r="R80" s="19"/>
+      <c r="S80" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" s="11" t="s">
         <v>87</v>
       </c>
@@ -4218,7 +4452,7 @@
         <v>44126</v>
       </c>
       <c r="G81" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>52</v>
       </c>
       <c r="H81" s="16" t="s">
@@ -4229,23 +4463,29 @@
       </c>
       <c r="J81" s="19"/>
       <c r="K81" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>364</v>
       </c>
-      <c r="M81" t="s">
+      <c r="L81" s="19"/>
+      <c r="M81" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="N81">
+      <c r="N81" s="19">
         <v>4</v>
       </c>
-      <c r="O81">
+      <c r="O81" s="19">
         <v>10</v>
       </c>
-      <c r="P81">
+      <c r="P81" s="19">
         <v>14</v>
       </c>
-    </row>
-    <row r="82" spans="1:16">
+      <c r="Q81" s="19">
+        <v>23</v>
+      </c>
+      <c r="R81" s="19"/>
+      <c r="S81" s="19"/>
+    </row>
+    <row r="82" spans="1:19">
       <c r="A82" s="11" t="s">
         <v>96</v>
       </c>
@@ -4265,7 +4505,7 @@
         <v>44141</v>
       </c>
       <c r="G82" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>55.857142857142854</v>
       </c>
       <c r="H82" s="16" t="s">
@@ -4276,23 +4516,29 @@
       </c>
       <c r="J82" s="19"/>
       <c r="K82" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>391</v>
       </c>
-      <c r="M82" t="s">
+      <c r="L82" s="19"/>
+      <c r="M82" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="N82">
+      <c r="N82" s="19">
         <v>2</v>
       </c>
-      <c r="O82">
+      <c r="O82" s="19">
         <v>7</v>
       </c>
-      <c r="P82">
+      <c r="P82" s="19">
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:16">
+      <c r="Q82" s="19">
+        <v>24</v>
+      </c>
+      <c r="R82" s="19"/>
+      <c r="S82" s="19"/>
+    </row>
+    <row r="83" spans="1:19">
       <c r="A83" s="11" t="s">
         <v>98</v>
       </c>
@@ -4312,7 +4558,7 @@
         <v>44145</v>
       </c>
       <c r="G83" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>59.142857142857146</v>
       </c>
       <c r="H83" s="16" t="s">
@@ -4323,23 +4569,29 @@
       </c>
       <c r="J83" s="19"/>
       <c r="K83" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>414</v>
       </c>
-      <c r="M83" t="s">
+      <c r="L83" s="19"/>
+      <c r="M83" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="N83">
+      <c r="N83" s="19">
         <v>2</v>
       </c>
-      <c r="O83">
+      <c r="O83" s="19">
         <v>9</v>
       </c>
-      <c r="P83">
+      <c r="P83" s="19">
         <v>14</v>
       </c>
-    </row>
-    <row r="84" spans="1:16">
+      <c r="Q83" s="19">
+        <v>25</v>
+      </c>
+      <c r="R83" s="19"/>
+      <c r="S83" s="19"/>
+    </row>
+    <row r="84" spans="1:19">
       <c r="A84" s="11" t="s">
         <v>99</v>
       </c>
@@ -4359,7 +4611,7 @@
         <v>44145</v>
       </c>
       <c r="G84" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>60.285714285714285</v>
       </c>
       <c r="H84" s="16" t="s">
@@ -4370,23 +4622,29 @@
       </c>
       <c r="J84" s="19"/>
       <c r="K84" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>422</v>
       </c>
-      <c r="M84" t="s">
+      <c r="L84" s="19"/>
+      <c r="M84" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="N84">
+      <c r="N84" s="19">
         <v>2</v>
       </c>
-      <c r="O84">
+      <c r="O84" s="19">
         <v>8</v>
       </c>
-      <c r="P84">
+      <c r="P84" s="19">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:16">
+      <c r="Q84" s="19">
+        <v>26</v>
+      </c>
+      <c r="R84" s="19"/>
+      <c r="S84" s="19"/>
+    </row>
+    <row r="85" spans="1:19">
       <c r="A85" s="11" t="s">
         <v>110</v>
       </c>
@@ -4406,7 +4664,7 @@
         <v>44158</v>
       </c>
       <c r="G85" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>53.285714285714285</v>
       </c>
       <c r="H85" s="16" t="s">
@@ -4417,21 +4675,29 @@
       </c>
       <c r="J85" s="19"/>
       <c r="K85" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>373</v>
       </c>
-      <c r="M85" t="s">
+      <c r="L85" s="19"/>
+      <c r="M85" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="N85">
+      <c r="N85" s="19">
         <v>1</v>
       </c>
-      <c r="O85">
+      <c r="O85" s="19">
         <v>6</v>
       </c>
-      <c r="P85">
+      <c r="P85" s="19">
         <v>13</v>
       </c>
+      <c r="Q85" s="19">
+        <v>27</v>
+      </c>
+      <c r="R85" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="S85" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>

<commit_message>
changed SEM to SD
</commit_message>
<xml_diff>
--- a/init_Synopsis_Dbdb.xlsx
+++ b/init_Synopsis_Dbdb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ipzach\Documents\MATLAB\Diabetes-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922A9D68-A5AF-42E7-B9B9-E472EA90309E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045679DC-6B57-443C-900A-B6AF435B12FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1094,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="R53" sqref="R53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U76" sqref="U76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -3403,7 +3403,9 @@
       <c r="S61" s="54">
         <v>7</v>
       </c>
-      <c r="T61" s="54"/>
+      <c r="T61" s="54">
+        <v>7</v>
+      </c>
     </row>
     <row r="62" spans="1:20">
       <c r="A62" s="47" t="s">
@@ -3566,7 +3568,7 @@
       <c r="R64" s="54"/>
       <c r="S64" s="54"/>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:20">
       <c r="A65" s="47" t="s">
         <v>107</v>
       </c>
@@ -3619,7 +3621,7 @@
       <c r="R65" s="54"/>
       <c r="S65" s="54"/>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:20">
       <c r="A66" s="47" t="s">
         <v>111</v>
       </c>
@@ -3672,7 +3674,7 @@
       <c r="R66" s="54"/>
       <c r="S66" s="54"/>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:20">
       <c r="A67" s="47" t="s">
         <v>112</v>
       </c>
@@ -3725,7 +3727,7 @@
       <c r="R67" s="54"/>
       <c r="S67" s="54"/>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:20">
       <c r="A68" s="56" t="s">
         <v>37</v>
       </c>
@@ -3779,8 +3781,11 @@
       <c r="S68" s="64">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:19">
+      <c r="T68" s="64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" s="56" t="s">
         <v>38</v>
       </c>
@@ -3835,7 +3840,7 @@
       </c>
       <c r="S69" s="64"/>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:20">
       <c r="A70" s="56" t="s">
         <v>39</v>
       </c>
@@ -3890,7 +3895,7 @@
       </c>
       <c r="S70" s="64"/>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:20">
       <c r="A71" s="56" t="s">
         <v>90</v>
       </c>
@@ -3945,7 +3950,7 @@
       </c>
       <c r="S71" s="64"/>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:20">
       <c r="A72" s="56" t="s">
         <v>94</v>
       </c>
@@ -3998,7 +4003,7 @@
       <c r="R72" s="64"/>
       <c r="S72" s="64"/>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:20">
       <c r="A73" s="20" t="s">
         <v>51</v>
       </c>
@@ -4052,8 +4057,11 @@
       <c r="S73" s="27">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:19">
+      <c r="T73" s="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74" s="20" t="s">
         <v>52</v>
       </c>
@@ -4108,7 +4116,7 @@
       </c>
       <c r="S74" s="27"/>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:20">
       <c r="A75" s="20" t="s">
         <v>53</v>
       </c>
@@ -4163,7 +4171,7 @@
       </c>
       <c r="S75" s="27"/>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:20">
       <c r="A76" s="20" t="s">
         <v>57</v>
       </c>
@@ -4218,7 +4226,7 @@
       </c>
       <c r="S76" s="27"/>
     </row>
-    <row r="77" spans="1:19">
+    <row r="77" spans="1:20">
       <c r="A77" s="20" t="s">
         <v>58</v>
       </c>
@@ -4271,7 +4279,7 @@
       <c r="R77" s="27"/>
       <c r="S77" s="27"/>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:20">
       <c r="A78" s="20" t="s">
         <v>102</v>
       </c>
@@ -4324,7 +4332,7 @@
       <c r="R78" s="27"/>
       <c r="S78" s="27"/>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:20">
       <c r="A79" s="20" t="s">
         <v>103</v>
       </c>
@@ -4377,7 +4385,7 @@
       <c r="R79" s="27"/>
       <c r="S79" s="27"/>
     </row>
-    <row r="80" spans="1:19">
+    <row r="80" spans="1:20">
       <c r="A80" s="11" t="s">
         <v>84</v>
       </c>
@@ -4429,6 +4437,9 @@
       </c>
       <c r="R80" s="19"/>
       <c r="S80" s="19">
+        <v>6</v>
+      </c>
+      <c r="T80" s="19">
         <v>6</v>
       </c>
     </row>

</xml_diff>